<commit_message>
mds diogo, 1h da manhã
</commit_message>
<xml_diff>
--- a/Otimização/triagem.xlsx
+++ b/Otimização/triagem.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,25 +493,25 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>513.4663641264968</v>
+        <v>565.1923707142779</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45413.86063322327</v>
+        <v>45413.90750580061</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45413.86077197333</v>
+        <v>45413.907636235</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0.0001387500694444445</v>
+        <v>0.0001304343865740741</v>
       </c>
       <c r="G2" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H2" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I2" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -527,27 +527,299 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>797.9987147326889</v>
+        <v>703.9281400860115</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45413.86077254323</v>
+        <v>45413.90764671707</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45413.86077735396</v>
+        <v>45413.90765120689</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>4.810729166666666e-06</v>
+        <v>4.489814814814815e-06</v>
       </c>
       <c r="G3" t="n">
+        <v>14</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>744.2480782766445</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45413.90765201986</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45413.90765606792</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>4.048055555555555e-06</v>
+      </c>
+      <c r="G4" t="n">
+        <v>22</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>633.050001047896</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45413.9076567984</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45413.90766115845</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>4.360046296296296e-06</v>
+      </c>
+      <c r="G5" t="n">
         <v>23</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H5" t="n">
+        <v>21</v>
+      </c>
+      <c r="I5" t="n">
+        <v>13</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>567.1161762126092</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45413.90766198299</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>45413.9076662549</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>4.271909722222223e-06</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25</v>
+      </c>
+      <c r="H6" t="n">
+        <v>27</v>
+      </c>
+      <c r="I6" t="n">
+        <v>15</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>706.0405603478761</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45413.90766709617</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>45413.90767021354</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>3.117372685185185e-06</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I3" t="n">
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>631.2513793815023</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45413.90767076387</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>45413.90767342736</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>2.663483796296296e-06</v>
+      </c>
+      <c r="G8" t="n">
+        <v>26</v>
+      </c>
+      <c r="H8" t="n">
+        <v>25</v>
+      </c>
+      <c r="I8" t="n">
+        <v>21</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>643.3065150904984</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45413.90767412398</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45413.90767807258</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>3.948599537037037e-06</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>11</v>
+      </c>
+      <c r="I9" t="n">
+        <v>21</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>600.0418887143586</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45413.90767898317</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>45413.90768313344</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>4.150266203703703e-06</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8</v>
+      </c>
+      <c r="H10" t="n">
+        <v>12</v>
+      </c>
+      <c r="I10" t="n">
+        <v>17</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>744.8583513583845</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45413.90769887075</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45413.90770314227</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>4.271516203703704e-06</v>
+      </c>
+      <c r="G11" t="n">
+        <v>15</v>
+      </c>
+      <c r="H11" t="n">
+        <v>23</v>
+      </c>
+      <c r="I11" t="n">
+        <v>19</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>COMPLETE</t>
         </is>

</xml_diff>